<commit_message>
Update 4.0.1: Fix Fecha de comrpobante en formato de Excel + IF Tipo de Servicip
</commit_message>
<xml_diff>
--- a/Facturador_Windows/Archivo para hacer Facturas 3.0.xlsx
+++ b/Facturador_Windows/Archivo para hacer Facturas 3.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\BOT-Facturador-AFIP\Facturador_Windows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D289F68F-2249-4AD5-A9BB-B1F257B566BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E03AEA1-E980-4CF2-A228-F10FA1E148CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="71">
   <si>
     <t>Fecha</t>
   </si>
@@ -138,9 +138,6 @@
   </si>
   <si>
     <t>Aux unidades</t>
-  </si>
-  <si>
-    <t>11/11/2022</t>
   </si>
   <si>
     <t>Factura A</t>
@@ -907,7 +904,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -959,7 +956,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1163,10 +1160,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="K17" sqref="K17"/>
-      <selection pane="bottomLeft" activeCell="S2" sqref="S2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,32 +1297,32 @@
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>34</v>
+      <c r="A2" s="8">
+        <v>44992</v>
       </c>
       <c r="B2" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C2),MONTH(C2),1),"dd/mm/aaaa")</f>
-        <v>01/10/2022</v>
+        <f t="shared" ref="B2:B17" si="0">TEXT(DATE(YEAR(C2),MONTH(C2),1),"dd/mm/aaaa")</f>
+        <v>01/02/2023</v>
       </c>
       <c r="C2" s="9" t="str">
-        <f>TEXT(EOMONTH(A2,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" ref="C2:C17" si="1">TEXT(EOMONTH(A2,-1),"dd/mm/aaaa")</f>
+        <v>28/02/2023</v>
       </c>
       <c r="D2" s="9" t="str">
-        <f>TEXT(A2+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" ref="D2:D17" si="2">TEXT(A2+14,"dd/mm/aaaa")</f>
+        <v>21/03/2023</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>9</v>
@@ -1334,11 +1331,11 @@
         <v>33610006189</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L2" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B2,"mmmm"))</f>
-        <v>Honorarios Octubre</v>
+        <v>Honorarios Febrero</v>
       </c>
       <c r="M2" s="4">
         <v>5.04</v>
@@ -1350,18 +1347,18 @@
         <v>44628.1</v>
       </c>
       <c r="P2" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
       <c r="S2" s="11"/>
       <c r="T2" s="13"/>
       <c r="U2" s="1" t="str">
-        <f t="shared" ref="U2" si="0">TEXT(R2,"00000")</f>
+        <f t="shared" ref="U2" si="3">TEXT(R2,"00000")</f>
         <v>00000</v>
       </c>
       <c r="V2" s="1" t="str">
-        <f t="shared" ref="V2" si="1">TEXT(S2,"00000000")</f>
+        <f t="shared" ref="V2" si="4">TEXT(S2,"00000000")</f>
         <v>00000000</v>
       </c>
       <c r="W2" s="1" t="str">
@@ -1369,11 +1366,11 @@
         <v>00/01/YYYY</v>
       </c>
       <c r="X2" s="14">
-        <f t="shared" ref="X2" si="2">ROUND(O2*P2,2)</f>
+        <f t="shared" ref="X2" si="5">ROUND(O2*P2,2)</f>
         <v>9371.9</v>
       </c>
       <c r="Y2" s="14">
-        <f t="shared" ref="Y2" si="3">O2+X2</f>
+        <f t="shared" ref="Y2" si="6">O2+X2</f>
         <v>54000</v>
       </c>
       <c r="Z2" s="10" t="str">
@@ -1386,7 +1383,7 @@
       </c>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1">
-        <f t="shared" ref="AC2" si="4">ROW(K2)</f>
+        <f t="shared" ref="AC2" si="7">ROW(K2)</f>
         <v>2</v>
       </c>
       <c r="AD2" s="1" t="str">
@@ -1394,45 +1391,45 @@
         <v>33610006189-1</v>
       </c>
       <c r="AF2" s="15">
-        <f t="shared" ref="AF2" si="5">CEILING(N2*M2*(1+P2),500)</f>
+        <f t="shared" ref="AF2" si="8">CEILING(N2*M2*(1+P2),500)</f>
         <v>54000</v>
       </c>
       <c r="AG2" s="15">
-        <f t="shared" ref="AG2" si="6">ROUND((AF2/(1+P2)),2)</f>
+        <f t="shared" ref="AG2" si="9">ROUND((AF2/(1+P2)),2)</f>
         <v>44628.1</v>
       </c>
       <c r="AH2" s="16">
-        <f t="shared" ref="AH2" si="7">ROUND(AG2/N2,4)</f>
+        <f t="shared" ref="AH2" si="10">ROUND(AG2/N2,4)</f>
         <v>5.0419</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>34</v>
+      <c r="A3" s="8">
+        <v>44992</v>
       </c>
       <c r="B3" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C3),MONTH(C3),1),"dd/mm/aaaa")</f>
-        <v>01/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>01/02/2023</v>
       </c>
       <c r="C3" s="9" t="str">
-        <f>TEXT(EOMONTH(A3,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="1"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D3" s="9" t="str">
-        <f>TEXT(A3+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="2"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>9</v>
@@ -1441,10 +1438,10 @@
         <v>33610006189</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M3" s="4">
         <v>5.04</v>
@@ -1456,43 +1453,43 @@
         <v>44628.1</v>
       </c>
       <c r="P3" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
       <c r="T3" s="13"/>
       <c r="U3" s="1" t="str">
-        <f t="shared" ref="U3:U17" si="8">TEXT(R3,"00000")</f>
+        <f t="shared" ref="U3:U17" si="11">TEXT(R3,"00000")</f>
         <v>00000</v>
       </c>
       <c r="V3" s="1" t="str">
-        <f t="shared" ref="V3:V17" si="9">TEXT(S3,"00000000")</f>
+        <f t="shared" ref="V3:V17" si="12">TEXT(S3,"00000000")</f>
         <v>00000000</v>
       </c>
       <c r="W3" s="1" t="str">
-        <f t="shared" ref="W3:W17" si="10">TEXT(T3,"DD/MM/YYYY")</f>
+        <f t="shared" ref="W3:W17" si="13">TEXT(T3,"DD/MM/YYYY")</f>
         <v>00/01/YYYY</v>
       </c>
       <c r="X3" s="14">
-        <f t="shared" ref="X3:X17" si="11">ROUND(O3*P3,2)</f>
+        <f t="shared" ref="X3:X17" si="14">ROUND(O3*P3,2)</f>
         <v>9371.9</v>
       </c>
       <c r="Y3" s="14">
-        <f t="shared" ref="Y3:Y17" si="12">O3+X3</f>
+        <f t="shared" ref="Y3:Y17" si="15">O3+X3</f>
         <v>54000</v>
       </c>
       <c r="Z3" s="10" t="str">
-        <f t="shared" ref="Z3:Z17" si="13">IF(F3="Factura A",SUBSTITUTE(TEXT(O3,"0.00"),",","."),SUBSTITUTE(TEXT(Y3,"0.00"),",","."))</f>
+        <f t="shared" ref="Z3:Z17" si="16">IF(F3="Factura A",SUBSTITUTE(TEXT(O3,"0.00"),",","."),SUBSTITUTE(TEXT(Y3,"0.00"),",","."))</f>
         <v>44.628</v>
       </c>
       <c r="AA3" s="10" t="str">
-        <f t="shared" ref="AA3:AA17" si="14">SUBSTITUTE(TEXT(ROUNDUP(Y3,0)-Y3,"0.00"),",",".")</f>
+        <f t="shared" ref="AA3:AA17" si="17">SUBSTITUTE(TEXT(ROUNDUP(Y3,0)-Y3,"0.00"),",",".")</f>
         <v>000</v>
       </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1">
-        <f t="shared" ref="AC3:AC17" si="15">ROW(K3)</f>
+        <f t="shared" ref="AC3:AC17" si="18">ROW(K3)</f>
         <v>3</v>
       </c>
       <c r="AD3" s="1" t="str">
@@ -1500,45 +1497,45 @@
         <v>33610006189-2</v>
       </c>
       <c r="AF3" s="15">
-        <f t="shared" ref="AF3:AF17" si="16">CEILING(N3*M3*(1+P3),500)</f>
+        <f t="shared" ref="AF3:AF17" si="19">CEILING(N3*M3*(1+P3),500)</f>
         <v>54000</v>
       </c>
       <c r="AG3" s="15">
-        <f t="shared" ref="AG3:AG17" si="17">ROUND((AF3/(1+P3)),2)</f>
+        <f t="shared" ref="AG3:AG17" si="20">ROUND((AF3/(1+P3)),2)</f>
         <v>44628.1</v>
       </c>
       <c r="AH3" s="16">
-        <f t="shared" ref="AH3:AH17" si="18">ROUND(AG3/N3,4)</f>
+        <f t="shared" ref="AH3:AH17" si="21">ROUND(AG3/N3,4)</f>
         <v>5.0419</v>
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>34</v>
+      <c r="A4" s="8">
+        <v>44992</v>
       </c>
       <c r="B4" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C4),MONTH(C4),1),"dd/mm/aaaa")</f>
-        <v>01/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>01/02/2023</v>
       </c>
       <c r="C4" s="9" t="str">
-        <f>TEXT(EOMONTH(A4,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="1"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D4" s="9" t="str">
-        <f>TEXT(A4+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="2"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>9</v>
@@ -1547,11 +1544,11 @@
         <v>30610252334</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L4" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B4,"mmmm"))</f>
-        <v>Honorarios Octubre</v>
+        <v>Honorarios Febrero</v>
       </c>
       <c r="M4" s="4">
         <v>10.039999999999999</v>
@@ -1563,43 +1560,43 @@
         <v>88842.97</v>
       </c>
       <c r="P4" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
       <c r="S4" s="11"/>
       <c r="T4" s="13"/>
       <c r="U4" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>00000</v>
       </c>
       <c r="V4" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000000</v>
       </c>
       <c r="W4" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="X4" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>18657.02</v>
       </c>
       <c r="Y4" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>107499.99</v>
       </c>
       <c r="Z4" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>88.843</v>
       </c>
       <c r="AA4" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="AD4" s="1" t="str">
@@ -1607,45 +1604,45 @@
         <v>30610252334-1</v>
       </c>
       <c r="AF4" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>108000</v>
       </c>
       <c r="AG4" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>89256.2</v>
       </c>
       <c r="AH4" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>10.0837</v>
       </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>34</v>
+      <c r="A5" s="8">
+        <v>44992</v>
       </c>
       <c r="B5" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C5),MONTH(C5),1),"dd/mm/aaaa")</f>
-        <v>01/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>01/02/2023</v>
       </c>
       <c r="C5" s="9" t="str">
-        <f>TEXT(EOMONTH(A5,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="1"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D5" s="9" t="str">
-        <f>TEXT(A5+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="2"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>9</v>
@@ -1654,10 +1651,10 @@
         <v>30684125792</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="M5" s="4">
         <v>7</v>
@@ -1669,51 +1666,51 @@
         <v>61983.47</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R5" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S5" s="11" t="s">
         <v>47</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>48</v>
       </c>
       <c r="T5" s="13">
         <v>44816</v>
       </c>
       <c r="U5" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>00002</v>
       </c>
       <c r="V5" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000150</v>
       </c>
       <c r="W5" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>12/09/YYYY</v>
       </c>
       <c r="X5" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>13016.53</v>
       </c>
       <c r="Y5" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>75000</v>
       </c>
       <c r="Z5" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>75.000</v>
       </c>
       <c r="AA5" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="AD5" s="1" t="str">
@@ -1721,45 +1718,45 @@
         <v>30684125792-1</v>
       </c>
       <c r="AF5" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>75000</v>
       </c>
       <c r="AG5" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>61983.47</v>
       </c>
       <c r="AH5" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>7.0026000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>34</v>
+      <c r="A6" s="8">
+        <v>44992</v>
       </c>
       <c r="B6" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C6),MONTH(C6),1),"dd/mm/aaaa")</f>
-        <v>01/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>01/02/2023</v>
       </c>
       <c r="C6" s="9" t="str">
-        <f>TEXT(EOMONTH(A6,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="1"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D6" s="9" t="str">
-        <f>TEXT(A6+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="2"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>9</v>
@@ -1768,10 +1765,10 @@
         <v>30684125792</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="M6" s="4">
         <v>7</v>
@@ -1783,51 +1780,51 @@
         <v>61983.47</v>
       </c>
       <c r="P6" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="R6" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="S6" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="T6" s="13">
         <v>44816</v>
       </c>
       <c r="U6" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>00002</v>
       </c>
       <c r="V6" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000151</v>
       </c>
       <c r="W6" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>12/09/YYYY</v>
       </c>
       <c r="X6" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>13016.53</v>
       </c>
       <c r="Y6" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>75000</v>
       </c>
       <c r="Z6" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>75.000</v>
       </c>
       <c r="AA6" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="AD6" s="1" t="str">
@@ -1835,45 +1832,45 @@
         <v>30684125792-2</v>
       </c>
       <c r="AF6" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>75000</v>
       </c>
       <c r="AG6" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>61983.47</v>
       </c>
       <c r="AH6" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>7.0026000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>34</v>
+      <c r="A7" s="8">
+        <v>44992</v>
       </c>
       <c r="B7" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C7),MONTH(C7),1),"dd/mm/aaaa")</f>
-        <v>01/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>01/02/2023</v>
       </c>
       <c r="C7" s="9" t="str">
-        <f>TEXT(EOMONTH(A7,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="1"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D7" s="9" t="str">
-        <f>TEXT(A7+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="2"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>9</v>
@@ -1882,11 +1879,11 @@
         <v>30525733870</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L7" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B7,"mmmm"))</f>
-        <v>Honorarios Octubre</v>
+        <v>Honorarios Febrero</v>
       </c>
       <c r="M7" s="4">
         <v>8.0299999999999994</v>
@@ -1898,43 +1895,43 @@
         <v>71074.38</v>
       </c>
       <c r="P7" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
       <c r="T7" s="13"/>
       <c r="U7" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>00000</v>
       </c>
       <c r="V7" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000000</v>
       </c>
       <c r="W7" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="X7" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>14925.62</v>
       </c>
       <c r="Y7" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>86000</v>
       </c>
       <c r="Z7" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>71.074</v>
       </c>
       <c r="AA7" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>7</v>
       </c>
       <c r="AD7" s="1" t="str">
@@ -1942,45 +1939,45 @@
         <v>30525733870-1</v>
       </c>
       <c r="AF7" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>86500</v>
       </c>
       <c r="AG7" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>71487.600000000006</v>
       </c>
       <c r="AH7" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>8.0762999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>34</v>
+      <c r="A8" s="8">
+        <v>44992</v>
       </c>
       <c r="B8" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C8),MONTH(C8),1),"dd/mm/aaaa")</f>
-        <v>01/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>01/02/2023</v>
       </c>
       <c r="C8" s="9" t="str">
-        <f>TEXT(EOMONTH(A8,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="1"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D8" s="9" t="str">
-        <f>TEXT(A8+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="2"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>9</v>
@@ -1989,11 +1986,11 @@
         <v>30710964277</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L8" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
-        <v>Honorarios Octubre</v>
+        <v>Honorarios Febrero</v>
       </c>
       <c r="M8" s="4">
         <v>9.01</v>
@@ -2005,43 +2002,43 @@
         <v>79752.070000000007</v>
       </c>
       <c r="P8" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
       <c r="T8" s="13"/>
       <c r="U8" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>00000</v>
       </c>
       <c r="V8" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000000</v>
       </c>
       <c r="W8" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="X8" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>16747.93</v>
       </c>
       <c r="Y8" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>96500</v>
       </c>
       <c r="Z8" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>79.752</v>
       </c>
       <c r="AA8" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>8</v>
       </c>
       <c r="AD8" s="1" t="str">
@@ -2049,45 +2046,45 @@
         <v>30710964277-1</v>
       </c>
       <c r="AF8" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>97000</v>
       </c>
       <c r="AG8" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>80165.289999999994</v>
       </c>
       <c r="AH8" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>9.0566999999999993</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>34</v>
+      <c r="A9" s="8">
+        <v>44992</v>
       </c>
       <c r="B9" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C9),MONTH(C9),1),"dd/mm/aaaa")</f>
-        <v>01/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>01/02/2023</v>
       </c>
       <c r="C9" s="9" t="str">
-        <f>TEXT(EOMONTH(A9,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="1"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D9" s="9" t="str">
-        <f>TEXT(A9+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="2"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>9</v>
@@ -2096,11 +2093,11 @@
         <v>33615420269</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L9" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B9,"mmmm"))</f>
-        <v>Honorarios Octubre</v>
+        <v>Honorarios Febrero</v>
       </c>
       <c r="M9" s="4">
         <v>10.039999999999999</v>
@@ -2112,43 +2109,43 @@
         <v>88842.97</v>
       </c>
       <c r="P9" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q9" s="11"/>
       <c r="R9" s="11"/>
       <c r="S9" s="11"/>
       <c r="T9" s="13"/>
       <c r="U9" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>00000</v>
       </c>
       <c r="V9" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000000</v>
       </c>
       <c r="W9" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="X9" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>18657.02</v>
       </c>
       <c r="Y9" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>107499.99</v>
       </c>
       <c r="Z9" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>88.843</v>
       </c>
       <c r="AA9" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="AD9" s="1" t="str">
@@ -2156,45 +2153,45 @@
         <v>33615420269-1</v>
       </c>
       <c r="AF9" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>108000</v>
       </c>
       <c r="AG9" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>89256.2</v>
       </c>
       <c r="AH9" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>10.0837</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>34</v>
+      <c r="A10" s="8">
+        <v>44992</v>
       </c>
       <c r="B10" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C10),MONTH(C10),1),"dd/mm/aaaa")</f>
-        <v>01/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>01/02/2023</v>
       </c>
       <c r="C10" s="9" t="str">
-        <f>TEXT(EOMONTH(A10,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="1"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D10" s="9" t="str">
-        <f>TEXT(A10+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="2"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>9</v>
@@ -2203,10 +2200,10 @@
         <v>30525390086</v>
       </c>
       <c r="K10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="M10" s="4">
         <v>9.01</v>
@@ -2218,43 +2215,43 @@
         <v>79752.070000000007</v>
       </c>
       <c r="P10" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q10" s="11"/>
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
       <c r="T10" s="13"/>
       <c r="U10" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>00000</v>
       </c>
       <c r="V10" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000000</v>
       </c>
       <c r="W10" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="X10" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>16747.93</v>
       </c>
       <c r="Y10" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>96500</v>
       </c>
       <c r="Z10" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>79.752</v>
       </c>
       <c r="AA10" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
       <c r="AD10" s="1" t="str">
@@ -2262,45 +2259,45 @@
         <v>30525390086-1</v>
       </c>
       <c r="AF10" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>97000</v>
       </c>
       <c r="AG10" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>80165.289999999994</v>
       </c>
       <c r="AH10" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>9.0566999999999993</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>34</v>
+      <c r="A11" s="8">
+        <v>44992</v>
       </c>
       <c r="B11" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C11),MONTH(C11),1),"dd/mm/aaaa")</f>
-        <v>01/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>01/02/2023</v>
       </c>
       <c r="C11" s="9" t="str">
-        <f>TEXT(EOMONTH(A11,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="1"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D11" s="9" t="str">
-        <f>TEXT(A11+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="2"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>9</v>
@@ -2309,11 +2306,11 @@
         <v>20374730429</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L11" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B11,"mmmm"))</f>
-        <v>Honorarios Octubre</v>
+        <v>Honorarios Febrero</v>
       </c>
       <c r="M11" s="4">
         <v>1.03</v>
@@ -2325,43 +2322,43 @@
         <v>9090.91</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
       <c r="T11" s="13"/>
       <c r="U11" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>00000</v>
       </c>
       <c r="V11" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000000</v>
       </c>
       <c r="W11" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="X11" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1909.09</v>
       </c>
       <c r="Y11" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>11000</v>
       </c>
       <c r="Z11" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>9.091</v>
       </c>
       <c r="AA11" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="AD11" s="1" t="str">
@@ -2369,45 +2366,45 @@
         <v>20374730429-1</v>
       </c>
       <c r="AF11" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>11500</v>
       </c>
       <c r="AG11" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>9504.1299999999992</v>
       </c>
       <c r="AH11" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1.0737000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>34</v>
+      <c r="A12" s="8">
+        <v>44992</v>
       </c>
       <c r="B12" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C12),MONTH(C12),1),"dd/mm/aaaa")</f>
-        <v>01/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>01/02/2023</v>
       </c>
       <c r="C12" s="9" t="str">
-        <f>TEXT(EOMONTH(A12,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="1"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D12" s="9" t="str">
-        <f>TEXT(A12+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="2"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>9</v>
@@ -2416,11 +2413,11 @@
         <v>20147130202</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L12" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B12,"mmmm"))</f>
-        <v>Honorarios Octubre</v>
+        <v>Honorarios Febrero</v>
       </c>
       <c r="M12" s="4">
         <v>1.03</v>
@@ -2432,43 +2429,43 @@
         <v>9090.91</v>
       </c>
       <c r="P12" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q12" s="11"/>
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
       <c r="T12" s="13"/>
       <c r="U12" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>00000</v>
       </c>
       <c r="V12" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000000</v>
       </c>
       <c r="W12" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="X12" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1909.09</v>
       </c>
       <c r="Y12" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>11000</v>
       </c>
       <c r="Z12" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>9.091</v>
       </c>
       <c r="AA12" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="AD12" s="1" t="str">
@@ -2476,45 +2473,45 @@
         <v>20147130202-1</v>
       </c>
       <c r="AF12" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>11500</v>
       </c>
       <c r="AG12" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>9504.1299999999992</v>
       </c>
       <c r="AH12" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1.0737000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>34</v>
+      <c r="A13" s="8">
+        <v>44992</v>
       </c>
       <c r="B13" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C13),MONTH(C13),1),"dd/mm/aaaa")</f>
-        <v>01/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>01/02/2023</v>
       </c>
       <c r="C13" s="9" t="str">
-        <f>TEXT(EOMONTH(A13,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="1"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D13" s="9" t="str">
-        <f>TEXT(A13+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="2"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E13" s="2">
         <v>2</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>9</v>
@@ -2523,11 +2520,11 @@
         <v>30707354719</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L13" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B13,"mmmm"))</f>
-        <v>Honorarios Octubre</v>
+        <v>Honorarios Febrero</v>
       </c>
       <c r="M13" s="4">
         <v>1.03</v>
@@ -2539,43 +2536,43 @@
         <v>9090.91</v>
       </c>
       <c r="P13" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
       <c r="T13" s="13"/>
       <c r="U13" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>00000</v>
       </c>
       <c r="V13" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000000</v>
       </c>
       <c r="W13" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="X13" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1909.09</v>
       </c>
       <c r="Y13" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>11000</v>
       </c>
       <c r="Z13" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>11.000</v>
       </c>
       <c r="AA13" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>13</v>
       </c>
       <c r="AD13" s="1" t="str">
@@ -2583,58 +2580,58 @@
         <v>30707354719-1</v>
       </c>
       <c r="AF13" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>11500</v>
       </c>
       <c r="AG13" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>9504.1299999999992</v>
       </c>
       <c r="AH13" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1.0737000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>34</v>
+      <c r="A14" s="8">
+        <v>44992</v>
       </c>
       <c r="B14" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C14),MONTH(C14),1),"dd/mm/aaaa")</f>
-        <v>01/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>01/02/2023</v>
       </c>
       <c r="C14" s="9" t="str">
-        <f>TEXT(EOMONTH(A14,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="1"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D14" s="9" t="str">
-        <f>TEXT(A14+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="2"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="J14" s="2">
         <v>37473042</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L14" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B14,"mmmm"))</f>
-        <v>Honorarios Octubre</v>
+        <v>Honorarios Febrero</v>
       </c>
       <c r="M14" s="4">
         <v>1.03</v>
@@ -2646,43 +2643,43 @@
         <v>9090.91</v>
       </c>
       <c r="P14" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
       <c r="S14" s="11"/>
       <c r="T14" s="13"/>
       <c r="U14" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>00000</v>
       </c>
       <c r="V14" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000000</v>
       </c>
       <c r="W14" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="X14" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1909.09</v>
       </c>
       <c r="Y14" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>11000</v>
       </c>
       <c r="Z14" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>11.000</v>
       </c>
       <c r="AA14" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="AD14" s="1" t="str">
@@ -2690,45 +2687,45 @@
         <v>37473042-1</v>
       </c>
       <c r="AF14" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>11500</v>
       </c>
       <c r="AG14" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>9504.1299999999992</v>
       </c>
       <c r="AH14" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1.0737000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>34</v>
+      <c r="A15" s="8">
+        <v>44992</v>
       </c>
       <c r="B15" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C15),MONTH(C15),1),"dd/mm/aaaa")</f>
-        <v>01/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>01/02/2023</v>
       </c>
       <c r="C15" s="9" t="str">
-        <f>TEXT(EOMONTH(A15,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="1"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D15" s="9" t="str">
-        <f>TEXT(A15+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="2"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>9</v>
@@ -2737,10 +2734,10 @@
         <v>30707354719</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M15" s="4">
         <v>1.03</v>
@@ -2752,51 +2749,51 @@
         <v>9090.91</v>
       </c>
       <c r="P15" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q15" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R15" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S15" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T15" s="13">
         <v>44816</v>
       </c>
       <c r="U15" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>00002</v>
       </c>
       <c r="V15" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000152</v>
       </c>
       <c r="W15" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>12/09/YYYY</v>
       </c>
       <c r="X15" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1909.09</v>
       </c>
       <c r="Y15" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>11000</v>
       </c>
       <c r="Z15" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>11.000</v>
       </c>
       <c r="AA15" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>15</v>
       </c>
       <c r="AD15" s="1" t="str">
@@ -2804,57 +2801,57 @@
         <v>30707354719-2</v>
       </c>
       <c r="AF15" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>11500</v>
       </c>
       <c r="AG15" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>9504.1299999999992</v>
       </c>
       <c r="AH15" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1.0737000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>34</v>
+      <c r="A16" s="8">
+        <v>44992</v>
       </c>
       <c r="B16" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C16),MONTH(C16),1),"dd/mm/aaaa")</f>
-        <v>01/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>01/02/2023</v>
       </c>
       <c r="C16" s="9" t="str">
-        <f>TEXT(EOMONTH(A16,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="1"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D16" s="9" t="str">
-        <f>TEXT(A16+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="2"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="J16" s="2">
         <v>37473042</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M16" s="4">
         <v>1.03</v>
@@ -2866,51 +2863,51 @@
         <v>9090.91</v>
       </c>
       <c r="P16" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q16" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="R16" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S16" s="11" t="s">
         <v>68</v>
-      </c>
-      <c r="R16" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="S16" s="11" t="s">
-        <v>69</v>
       </c>
       <c r="T16" s="13">
         <v>44816</v>
       </c>
       <c r="U16" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>00002</v>
       </c>
       <c r="V16" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000153</v>
       </c>
       <c r="W16" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>12/09/YYYY</v>
       </c>
       <c r="X16" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1909.09</v>
       </c>
       <c r="Y16" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>11000</v>
       </c>
       <c r="Z16" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>11.000</v>
       </c>
       <c r="AA16" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="AD16" s="1" t="str">
@@ -2918,56 +2915,56 @@
         <v>37473042-2</v>
       </c>
       <c r="AF16" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>11500</v>
       </c>
       <c r="AG16" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>9504.1299999999992</v>
       </c>
       <c r="AH16" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1.0737000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>34</v>
+      <c r="A17" s="8">
+        <v>44992</v>
       </c>
       <c r="B17" s="9" t="str">
-        <f>TEXT(DATE(YEAR(C17),MONTH(C17),1),"dd/mm/aaaa")</f>
-        <v>01/10/2022</v>
+        <f t="shared" si="0"/>
+        <v>01/02/2023</v>
       </c>
       <c r="C17" s="9" t="str">
-        <f>TEXT(EOMONTH(A17,-1),"dd/mm/aaaa")</f>
-        <v>31/10/2022</v>
+        <f t="shared" si="1"/>
+        <v>28/02/2023</v>
       </c>
       <c r="D17" s="9" t="str">
-        <f>TEXT(A17+14,"dd/mm/aaaa")</f>
-        <v>25/11/2022</v>
+        <f t="shared" si="2"/>
+        <v>21/03/2023</v>
       </c>
       <c r="E17" s="2">
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L17" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B17,"mmmm"))</f>
-        <v>Honorarios Octubre</v>
+        <v>Honorarios Febrero</v>
       </c>
       <c r="M17" s="4">
         <v>1.03</v>
@@ -2979,43 +2976,43 @@
         <v>0</v>
       </c>
       <c r="P17" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q17" s="11"/>
       <c r="R17" s="11"/>
       <c r="S17" s="11"/>
       <c r="T17" s="13"/>
       <c r="U17" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>00000</v>
       </c>
       <c r="V17" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>00000000</v>
       </c>
       <c r="W17" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>00/01/YYYY</v>
       </c>
       <c r="X17" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Y17" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Z17" s="10" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>000</v>
       </c>
       <c r="AA17" s="10" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>000</v>
       </c>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>17</v>
       </c>
       <c r="AD17" s="1" t="str">
@@ -3023,15 +3020,15 @@
         <v>-0</v>
       </c>
       <c r="AF17" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>11500</v>
       </c>
       <c r="AG17" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="20"/>
         <v>9504.1299999999992</v>
       </c>
       <c r="AH17" s="16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>1.0737000000000001</v>
       </c>
     </row>

</xml_diff>